<commit_message>
Final Demo Commit-1: 12 Sep 2024
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Amitha_JavaPgms\Eclipse-Pgms\7rmartsupermarket\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9EB451-E93C-4C34-9F0D-64038374E368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D85F200-1AF7-4429-A1F1-A50983B8FED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="6" xr2:uid="{C6246969-9258-48DA-9497-6C98DB234FDD}"/>
+    <workbookView xWindow="5316" yWindow="2328" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="3" xr2:uid="{C6246969-9258-48DA-9497-6C98DB234FDD}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -108,9 +108,6 @@
     <t>Edit User Passwords</t>
   </si>
   <si>
-    <t>Arya Sug</t>
-  </si>
-  <si>
     <t>Anu Sud</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>HN: 24, Apex Building, Edappally</t>
+  </si>
+  <si>
+    <t>Arya Sugathan</t>
   </si>
 </sst>
 </file>
@@ -186,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -204,7 +204,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -910,14 +909,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DCDAA92-80CA-4E01-A750-EE56F9347265}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -942,10 +942,10 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -956,10 +956,10 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
         <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1050,7 +1050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852A3EEA-369D-487A-9E67-61F2CA2D1067}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
@@ -1063,21 +1063,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
       </c>
       <c r="C2">
         <v>9999999999</v>

</xml_diff>